<commit_message>
Converted to Maven Project. Added TestNG class
</commit_message>
<xml_diff>
--- a/stakeOverflow/bin/dataEngine/TestData1.xlsx
+++ b/stakeOverflow/bin/dataEngine/TestData1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>